<commit_message>
cambio de planillas completo
</commit_message>
<xml_diff>
--- a/src/assets/Test-Reporte_Elanco/nuevas/Ceres_eficacia_hex.xlsx
+++ b/src/assets/Test-Reporte_Elanco/nuevas/Ceres_eficacia_hex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elancoah-my.sharepoint.com/personal/patricio_pena_network_elancoah_com/Documents/TS - Imvixa/_Clientes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catta\Documents\COMPSCI\repos\elanco-infome-imvixa\src\assets\Test-Reporte_Elanco\nuevas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_9F4EF32E0039E894182426FA5F79D10FE27D1A0F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75A88DD-7DB5-4EC7-81FA-45666CC92333}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50711314-C60A-4ADC-AC62-E25867C7C35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -280,7 +280,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +580,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>